<commit_message>
correct transcription error for Romania
</commit_message>
<xml_diff>
--- a/semi_final_2_2022.xlsx
+++ b/semi_final_2_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Dropbox/Sheffield/Data/eurovision_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEA8D0D-AF86-EF47-B5E2-3FFA888480CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ECF9AB-16AA-7843-9967-B98124378E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" firstSheet="8" activeTab="20" xr2:uid="{EB7F70B0-9F3D-6443-8E8B-EA2FD7A7CE76}"/>
+    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" firstSheet="8" activeTab="15" xr2:uid="{EB7F70B0-9F3D-6443-8E8B-EA2FD7A7CE76}"/>
   </bookViews>
   <sheets>
     <sheet name="Australia" sheetId="1" r:id="rId1"/>
@@ -8665,6 +8665,372 @@
         <a:xfrm>
           <a:off x="0" y="3175000"/>
           <a:ext cx="406400" cy="431800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25" descr="🇧🇪">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1982E33E-D4E7-6B44-A7B0-CCC190CA5848}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2260600"/>
+          <a:ext cx="406400" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26" descr="🇪🇪">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B100CD1C-AC59-F742-9060-4E0A872EC2E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2260600"/>
+          <a:ext cx="406400" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27" descr="🇫🇮">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00F11176-3F3C-0944-8070-1916236CFC40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2489200"/>
+          <a:ext cx="406400" cy="431800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28" descr="🇲🇪">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C791720-6DE5-264A-AD6B-D42324A43493}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2260600"/>
+          <a:ext cx="406400" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29" descr="🇲🇰">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F682D8A-7337-C049-94B9-C36F05BAE5C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2489200"/>
+          <a:ext cx="406400" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30" descr="🇦🇺">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF9859D8-2B74-1944-9D31-DC95051A81AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2489200"/>
+          <a:ext cx="406400" cy="406400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -25260,7 +25626,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25416,8 +25782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7541B7A2-74D4-5E4D-9C4D-995929E97B2F}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25539,15 +25905,15 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -27406,7 +27772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736BAFBB-786B-DF48-80A5-D226C66CDC8C}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:I19"/>
     </sheetView>
   </sheetViews>

</xml_diff>